<commit_message>
Add HETD as input to FT-*HET
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A05730E-7638-45B5-8D8E-98314114E676}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4A7955-DCC7-4BF4-86FD-C5F6FB3DA609}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TRA-BLENDS" sheetId="17" r:id="rId1"/>
-    <sheet name="Regions" sheetId="15" r:id="rId2"/>
+    <sheet name="Regions" sheetId="15" r:id="rId1"/>
+    <sheet name="HET" sheetId="19" r:id="rId2"/>
     <sheet name="TRA" sheetId="2" r:id="rId3"/>
     <sheet name="UCT_TRA" sheetId="18" r:id="rId4"/>
     <sheet name="UPD_biogas" sheetId="11" r:id="rId5"/>
@@ -23,19 +23,19 @@
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
-    <definedName name="aa" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec2" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec3" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elecc" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="table6" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="124">
   <si>
     <t>UC_N</t>
   </si>
@@ -469,66 +469,9 @@
     <t>Kerosene</t>
   </si>
   <si>
-    <t>BASE</t>
-  </si>
-  <si>
     <t>SHARE-I</t>
   </si>
   <si>
-    <t>scenario</t>
-  </si>
-  <si>
-    <t>attribute</t>
-  </si>
-  <si>
-    <t>process</t>
-  </si>
-  <si>
-    <t>commodity</t>
-  </si>
-  <si>
-    <t>lim_type</t>
-  </si>
-  <si>
-    <t>time_slice</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>commodity_group</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>stage</t>
-  </si>
-  <si>
-    <t>sow</t>
-  </si>
-  <si>
-    <t>TRABCNG_BLD</t>
-  </si>
-  <si>
-    <t>ANNUAL</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>TRABJK_BLD</t>
-  </si>
-  <si>
-    <t>TRADST_BLD</t>
-  </si>
-  <si>
-    <t>TRAE85_BLD</t>
-  </si>
-  <si>
-    <t>TRAGSL_BLD</t>
-  </si>
-  <si>
     <t>~TFM_INS</t>
   </si>
   <si>
@@ -542,6 +485,12 @@
   </si>
   <si>
     <t>T-OTH_NEW</t>
+  </si>
+  <si>
+    <t>FT-*HET</t>
+  </si>
+  <si>
+    <t>HETD</t>
   </si>
 </sst>
 </file>
@@ -1177,1963 +1126,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D84E4A-22F2-4E71-B908-2FF7EAFC1BC6}">
-  <dimension ref="A1:L51"/>
-  <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42:L44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K1" t="s">
-        <v>128</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2">
-        <v>2018</v>
-      </c>
-      <c r="H2" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3">
-        <v>2020</v>
-      </c>
-      <c r="H3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" t="s">
-        <v>131</v>
-      </c>
-      <c r="J3" t="s">
-        <v>131</v>
-      </c>
-      <c r="K3" t="s">
-        <v>131</v>
-      </c>
-      <c r="L3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G4">
-        <v>2030</v>
-      </c>
-      <c r="H4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I4" t="s">
-        <v>131</v>
-      </c>
-      <c r="J4" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" t="s">
-        <v>131</v>
-      </c>
-      <c r="L4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5">
-        <v>2040</v>
-      </c>
-      <c r="H5" t="s">
-        <v>125</v>
-      </c>
-      <c r="I5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J5" t="s">
-        <v>131</v>
-      </c>
-      <c r="K5" t="s">
-        <v>131</v>
-      </c>
-      <c r="L5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6">
-        <v>2050</v>
-      </c>
-      <c r="H6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I6" t="s">
-        <v>131</v>
-      </c>
-      <c r="J6" t="s">
-        <v>131</v>
-      </c>
-      <c r="K6" t="s">
-        <v>131</v>
-      </c>
-      <c r="L6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7">
-        <v>2018</v>
-      </c>
-      <c r="H7" t="s">
-        <v>125</v>
-      </c>
-      <c r="I7" t="s">
-        <v>131</v>
-      </c>
-      <c r="J7" t="s">
-        <v>131</v>
-      </c>
-      <c r="K7" t="s">
-        <v>131</v>
-      </c>
-      <c r="L7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G8">
-        <v>2020</v>
-      </c>
-      <c r="H8" t="s">
-        <v>125</v>
-      </c>
-      <c r="I8" t="s">
-        <v>131</v>
-      </c>
-      <c r="J8" t="s">
-        <v>131</v>
-      </c>
-      <c r="K8" t="s">
-        <v>131</v>
-      </c>
-      <c r="L8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9">
-        <v>2030</v>
-      </c>
-      <c r="H9" t="s">
-        <v>125</v>
-      </c>
-      <c r="I9" t="s">
-        <v>131</v>
-      </c>
-      <c r="J9" t="s">
-        <v>131</v>
-      </c>
-      <c r="K9" t="s">
-        <v>131</v>
-      </c>
-      <c r="L9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G10">
-        <v>2040</v>
-      </c>
-      <c r="H10" t="s">
-        <v>125</v>
-      </c>
-      <c r="I10" t="s">
-        <v>131</v>
-      </c>
-      <c r="J10" t="s">
-        <v>131</v>
-      </c>
-      <c r="K10" t="s">
-        <v>131</v>
-      </c>
-      <c r="L10">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G11">
-        <v>2050</v>
-      </c>
-      <c r="H11" t="s">
-        <v>125</v>
-      </c>
-      <c r="I11" t="s">
-        <v>131</v>
-      </c>
-      <c r="J11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K11" t="s">
-        <v>131</v>
-      </c>
-      <c r="L11">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" t="s">
-        <v>130</v>
-      </c>
-      <c r="G12">
-        <v>2018</v>
-      </c>
-      <c r="H12" t="s">
-        <v>125</v>
-      </c>
-      <c r="I12" t="s">
-        <v>131</v>
-      </c>
-      <c r="J12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K12" t="s">
-        <v>131</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13">
-        <v>2020</v>
-      </c>
-      <c r="H13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I13" t="s">
-        <v>131</v>
-      </c>
-      <c r="J13" t="s">
-        <v>131</v>
-      </c>
-      <c r="K13" t="s">
-        <v>131</v>
-      </c>
-      <c r="L13">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" t="s">
-        <v>130</v>
-      </c>
-      <c r="G14">
-        <v>2030</v>
-      </c>
-      <c r="H14" t="s">
-        <v>125</v>
-      </c>
-      <c r="I14" t="s">
-        <v>131</v>
-      </c>
-      <c r="J14" t="s">
-        <v>131</v>
-      </c>
-      <c r="K14" t="s">
-        <v>131</v>
-      </c>
-      <c r="L14">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" t="s">
-        <v>130</v>
-      </c>
-      <c r="G15">
-        <v>2040</v>
-      </c>
-      <c r="H15" t="s">
-        <v>125</v>
-      </c>
-      <c r="I15" t="s">
-        <v>131</v>
-      </c>
-      <c r="J15" t="s">
-        <v>131</v>
-      </c>
-      <c r="K15" t="s">
-        <v>131</v>
-      </c>
-      <c r="L15">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" t="s">
-        <v>130</v>
-      </c>
-      <c r="G16">
-        <v>2050</v>
-      </c>
-      <c r="H16" t="s">
-        <v>125</v>
-      </c>
-      <c r="I16" t="s">
-        <v>131</v>
-      </c>
-      <c r="J16" t="s">
-        <v>131</v>
-      </c>
-      <c r="K16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L16">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F17" t="s">
-        <v>130</v>
-      </c>
-      <c r="G17">
-        <v>2018</v>
-      </c>
-      <c r="H17" t="s">
-        <v>125</v>
-      </c>
-      <c r="I17" t="s">
-        <v>131</v>
-      </c>
-      <c r="J17" t="s">
-        <v>131</v>
-      </c>
-      <c r="K17" t="s">
-        <v>131</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>116</v>
-      </c>
-      <c r="B18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" t="s">
-        <v>132</v>
-      </c>
-      <c r="D18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" t="s">
-        <v>130</v>
-      </c>
-      <c r="G18">
-        <v>2020</v>
-      </c>
-      <c r="H18" t="s">
-        <v>125</v>
-      </c>
-      <c r="I18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J18" t="s">
-        <v>131</v>
-      </c>
-      <c r="K18" t="s">
-        <v>131</v>
-      </c>
-      <c r="L18">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D19" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19">
-        <v>2030</v>
-      </c>
-      <c r="H19" t="s">
-        <v>125</v>
-      </c>
-      <c r="I19" t="s">
-        <v>131</v>
-      </c>
-      <c r="J19" t="s">
-        <v>131</v>
-      </c>
-      <c r="K19" t="s">
-        <v>131</v>
-      </c>
-      <c r="L19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" t="s">
-        <v>132</v>
-      </c>
-      <c r="D20" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" t="s">
-        <v>130</v>
-      </c>
-      <c r="G20">
-        <v>2040</v>
-      </c>
-      <c r="H20" t="s">
-        <v>125</v>
-      </c>
-      <c r="I20" t="s">
-        <v>131</v>
-      </c>
-      <c r="J20" t="s">
-        <v>131</v>
-      </c>
-      <c r="K20" t="s">
-        <v>131</v>
-      </c>
-      <c r="L20">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" t="s">
-        <v>132</v>
-      </c>
-      <c r="D21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" t="s">
-        <v>130</v>
-      </c>
-      <c r="G21">
-        <v>2050</v>
-      </c>
-      <c r="H21" t="s">
-        <v>125</v>
-      </c>
-      <c r="I21" t="s">
-        <v>131</v>
-      </c>
-      <c r="J21" t="s">
-        <v>131</v>
-      </c>
-      <c r="K21" t="s">
-        <v>131</v>
-      </c>
-      <c r="L21">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B22" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" t="s">
-        <v>133</v>
-      </c>
-      <c r="D22" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G22">
-        <v>2018</v>
-      </c>
-      <c r="H22" t="s">
-        <v>125</v>
-      </c>
-      <c r="I22" t="s">
-        <v>131</v>
-      </c>
-      <c r="J22" t="s">
-        <v>131</v>
-      </c>
-      <c r="K22" t="s">
-        <v>131</v>
-      </c>
-      <c r="L22">
-        <v>4.0877873467079801E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" t="s">
-        <v>133</v>
-      </c>
-      <c r="D23" t="s">
-        <v>95</v>
-      </c>
-      <c r="E23" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" t="s">
-        <v>130</v>
-      </c>
-      <c r="G23">
-        <v>2020</v>
-      </c>
-      <c r="H23" t="s">
-        <v>125</v>
-      </c>
-      <c r="I23" t="s">
-        <v>131</v>
-      </c>
-      <c r="J23" t="s">
-        <v>131</v>
-      </c>
-      <c r="K23" t="s">
-        <v>131</v>
-      </c>
-      <c r="L23">
-        <v>5.1152531327863002E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" t="s">
-        <v>133</v>
-      </c>
-      <c r="D24" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" t="s">
-        <v>130</v>
-      </c>
-      <c r="G24">
-        <v>2030</v>
-      </c>
-      <c r="H24" t="s">
-        <v>125</v>
-      </c>
-      <c r="I24" t="s">
-        <v>131</v>
-      </c>
-      <c r="J24" t="s">
-        <v>131</v>
-      </c>
-      <c r="K24" t="s">
-        <v>131</v>
-      </c>
-      <c r="L24">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" t="s">
-        <v>133</v>
-      </c>
-      <c r="D25" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" t="s">
-        <v>84</v>
-      </c>
-      <c r="F25" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25">
-        <v>2040</v>
-      </c>
-      <c r="H25" t="s">
-        <v>125</v>
-      </c>
-      <c r="I25" t="s">
-        <v>131</v>
-      </c>
-      <c r="J25" t="s">
-        <v>131</v>
-      </c>
-      <c r="K25" t="s">
-        <v>131</v>
-      </c>
-      <c r="L25">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>116</v>
-      </c>
-      <c r="B26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" t="s">
-        <v>133</v>
-      </c>
-      <c r="D26" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" t="s">
-        <v>130</v>
-      </c>
-      <c r="G26">
-        <v>2050</v>
-      </c>
-      <c r="H26" t="s">
-        <v>125</v>
-      </c>
-      <c r="I26" t="s">
-        <v>131</v>
-      </c>
-      <c r="J26" t="s">
-        <v>131</v>
-      </c>
-      <c r="K26" t="s">
-        <v>131</v>
-      </c>
-      <c r="L26">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>116</v>
-      </c>
-      <c r="B27" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" t="s">
-        <v>133</v>
-      </c>
-      <c r="D27" t="s">
-        <v>110</v>
-      </c>
-      <c r="E27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" t="s">
-        <v>130</v>
-      </c>
-      <c r="G27">
-        <v>2018</v>
-      </c>
-      <c r="H27" t="s">
-        <v>125</v>
-      </c>
-      <c r="I27" t="s">
-        <v>131</v>
-      </c>
-      <c r="J27" t="s">
-        <v>131</v>
-      </c>
-      <c r="K27" t="s">
-        <v>131</v>
-      </c>
-      <c r="L27">
-        <v>0.95912212653291995</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" t="s">
-        <v>133</v>
-      </c>
-      <c r="D28" t="s">
-        <v>110</v>
-      </c>
-      <c r="E28" t="s">
-        <v>84</v>
-      </c>
-      <c r="F28" t="s">
-        <v>130</v>
-      </c>
-      <c r="G28">
-        <v>2020</v>
-      </c>
-      <c r="H28" t="s">
-        <v>125</v>
-      </c>
-      <c r="I28" t="s">
-        <v>131</v>
-      </c>
-      <c r="J28" t="s">
-        <v>131</v>
-      </c>
-      <c r="K28" t="s">
-        <v>131</v>
-      </c>
-      <c r="L28">
-        <v>0.94884746867213698</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>116</v>
-      </c>
-      <c r="B29" t="s">
-        <v>117</v>
-      </c>
-      <c r="C29" t="s">
-        <v>133</v>
-      </c>
-      <c r="D29" t="s">
-        <v>110</v>
-      </c>
-      <c r="E29" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" t="s">
-        <v>130</v>
-      </c>
-      <c r="G29">
-        <v>2030</v>
-      </c>
-      <c r="H29" t="s">
-        <v>125</v>
-      </c>
-      <c r="I29" t="s">
-        <v>131</v>
-      </c>
-      <c r="J29" t="s">
-        <v>131</v>
-      </c>
-      <c r="K29" t="s">
-        <v>131</v>
-      </c>
-      <c r="L29">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" t="s">
-        <v>133</v>
-      </c>
-      <c r="D30" t="s">
-        <v>110</v>
-      </c>
-      <c r="E30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F30" t="s">
-        <v>130</v>
-      </c>
-      <c r="G30">
-        <v>2040</v>
-      </c>
-      <c r="H30" t="s">
-        <v>125</v>
-      </c>
-      <c r="I30" t="s">
-        <v>131</v>
-      </c>
-      <c r="J30" t="s">
-        <v>131</v>
-      </c>
-      <c r="K30" t="s">
-        <v>131</v>
-      </c>
-      <c r="L30">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" t="s">
-        <v>133</v>
-      </c>
-      <c r="D31" t="s">
-        <v>110</v>
-      </c>
-      <c r="E31" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" t="s">
-        <v>130</v>
-      </c>
-      <c r="G31">
-        <v>2050</v>
-      </c>
-      <c r="H31" t="s">
-        <v>125</v>
-      </c>
-      <c r="I31" t="s">
-        <v>131</v>
-      </c>
-      <c r="J31" t="s">
-        <v>131</v>
-      </c>
-      <c r="K31" t="s">
-        <v>131</v>
-      </c>
-      <c r="L31">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>116</v>
-      </c>
-      <c r="B32" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" t="s">
-        <v>134</v>
-      </c>
-      <c r="D32" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" t="s">
-        <v>130</v>
-      </c>
-      <c r="G32">
-        <v>2018</v>
-      </c>
-      <c r="H32" t="s">
-        <v>125</v>
-      </c>
-      <c r="I32" t="s">
-        <v>131</v>
-      </c>
-      <c r="J32" t="s">
-        <v>131</v>
-      </c>
-      <c r="K32" t="s">
-        <v>131</v>
-      </c>
-      <c r="L32">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>116</v>
-      </c>
-      <c r="B33" t="s">
-        <v>117</v>
-      </c>
-      <c r="C33" t="s">
-        <v>134</v>
-      </c>
-      <c r="D33" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" t="s">
-        <v>84</v>
-      </c>
-      <c r="F33" t="s">
-        <v>130</v>
-      </c>
-      <c r="G33">
-        <v>2020</v>
-      </c>
-      <c r="H33" t="s">
-        <v>125</v>
-      </c>
-      <c r="I33" t="s">
-        <v>131</v>
-      </c>
-      <c r="J33" t="s">
-        <v>131</v>
-      </c>
-      <c r="K33" t="s">
-        <v>131</v>
-      </c>
-      <c r="L33">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>116</v>
-      </c>
-      <c r="B34" t="s">
-        <v>117</v>
-      </c>
-      <c r="C34" t="s">
-        <v>134</v>
-      </c>
-      <c r="D34" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" t="s">
-        <v>84</v>
-      </c>
-      <c r="F34" t="s">
-        <v>130</v>
-      </c>
-      <c r="G34">
-        <v>2030</v>
-      </c>
-      <c r="H34" t="s">
-        <v>125</v>
-      </c>
-      <c r="I34" t="s">
-        <v>131</v>
-      </c>
-      <c r="J34" t="s">
-        <v>131</v>
-      </c>
-      <c r="K34" t="s">
-        <v>131</v>
-      </c>
-      <c r="L34">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>116</v>
-      </c>
-      <c r="B35" t="s">
-        <v>117</v>
-      </c>
-      <c r="C35" t="s">
-        <v>134</v>
-      </c>
-      <c r="D35" t="s">
-        <v>94</v>
-      </c>
-      <c r="E35" t="s">
-        <v>84</v>
-      </c>
-      <c r="F35" t="s">
-        <v>130</v>
-      </c>
-      <c r="G35">
-        <v>2040</v>
-      </c>
-      <c r="H35" t="s">
-        <v>125</v>
-      </c>
-      <c r="I35" t="s">
-        <v>131</v>
-      </c>
-      <c r="J35" t="s">
-        <v>131</v>
-      </c>
-      <c r="K35" t="s">
-        <v>131</v>
-      </c>
-      <c r="L35">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>116</v>
-      </c>
-      <c r="B36" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" t="s">
-        <v>134</v>
-      </c>
-      <c r="D36" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" t="s">
-        <v>84</v>
-      </c>
-      <c r="F36" t="s">
-        <v>130</v>
-      </c>
-      <c r="G36">
-        <v>2050</v>
-      </c>
-      <c r="H36" t="s">
-        <v>125</v>
-      </c>
-      <c r="I36" t="s">
-        <v>131</v>
-      </c>
-      <c r="J36" t="s">
-        <v>131</v>
-      </c>
-      <c r="K36" t="s">
-        <v>131</v>
-      </c>
-      <c r="L36">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>116</v>
-      </c>
-      <c r="B37" t="s">
-        <v>117</v>
-      </c>
-      <c r="C37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D37" t="s">
-        <v>102</v>
-      </c>
-      <c r="E37" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" t="s">
-        <v>130</v>
-      </c>
-      <c r="G37">
-        <v>2018</v>
-      </c>
-      <c r="H37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I37" t="s">
-        <v>131</v>
-      </c>
-      <c r="J37" t="s">
-        <v>131</v>
-      </c>
-      <c r="K37" t="s">
-        <v>131</v>
-      </c>
-      <c r="L37">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>116</v>
-      </c>
-      <c r="B38" t="s">
-        <v>117</v>
-      </c>
-      <c r="C38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D38" t="s">
-        <v>102</v>
-      </c>
-      <c r="E38" t="s">
-        <v>84</v>
-      </c>
-      <c r="F38" t="s">
-        <v>130</v>
-      </c>
-      <c r="G38">
-        <v>2020</v>
-      </c>
-      <c r="H38" t="s">
-        <v>125</v>
-      </c>
-      <c r="I38" t="s">
-        <v>131</v>
-      </c>
-      <c r="J38" t="s">
-        <v>131</v>
-      </c>
-      <c r="K38" t="s">
-        <v>131</v>
-      </c>
-      <c r="L38">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" t="s">
-        <v>117</v>
-      </c>
-      <c r="C39" t="s">
-        <v>134</v>
-      </c>
-      <c r="D39" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" t="s">
-        <v>130</v>
-      </c>
-      <c r="G39">
-        <v>2030</v>
-      </c>
-      <c r="H39" t="s">
-        <v>125</v>
-      </c>
-      <c r="I39" t="s">
-        <v>131</v>
-      </c>
-      <c r="J39" t="s">
-        <v>131</v>
-      </c>
-      <c r="K39" t="s">
-        <v>131</v>
-      </c>
-      <c r="L39">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>116</v>
-      </c>
-      <c r="B40" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D40" t="s">
-        <v>102</v>
-      </c>
-      <c r="E40" t="s">
-        <v>84</v>
-      </c>
-      <c r="F40" t="s">
-        <v>130</v>
-      </c>
-      <c r="G40">
-        <v>2040</v>
-      </c>
-      <c r="H40" t="s">
-        <v>125</v>
-      </c>
-      <c r="I40" t="s">
-        <v>131</v>
-      </c>
-      <c r="J40" t="s">
-        <v>131</v>
-      </c>
-      <c r="K40" t="s">
-        <v>131</v>
-      </c>
-      <c r="L40">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>116</v>
-      </c>
-      <c r="B41" t="s">
-        <v>117</v>
-      </c>
-      <c r="C41" t="s">
-        <v>134</v>
-      </c>
-      <c r="D41" t="s">
-        <v>102</v>
-      </c>
-      <c r="E41" t="s">
-        <v>84</v>
-      </c>
-      <c r="F41" t="s">
-        <v>130</v>
-      </c>
-      <c r="G41">
-        <v>2050</v>
-      </c>
-      <c r="H41" t="s">
-        <v>125</v>
-      </c>
-      <c r="I41" t="s">
-        <v>131</v>
-      </c>
-      <c r="J41" t="s">
-        <v>131</v>
-      </c>
-      <c r="K41" t="s">
-        <v>131</v>
-      </c>
-      <c r="L41">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>116</v>
-      </c>
-      <c r="B42" t="s">
-        <v>117</v>
-      </c>
-      <c r="C42" t="s">
-        <v>135</v>
-      </c>
-      <c r="D42" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" t="s">
-        <v>84</v>
-      </c>
-      <c r="F42" t="s">
-        <v>130</v>
-      </c>
-      <c r="G42">
-        <v>2018</v>
-      </c>
-      <c r="H42" t="s">
-        <v>125</v>
-      </c>
-      <c r="I42" t="s">
-        <v>131</v>
-      </c>
-      <c r="J42" t="s">
-        <v>131</v>
-      </c>
-      <c r="K42" t="s">
-        <v>131</v>
-      </c>
-      <c r="L42">
-        <v>4.5158565381788203E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>116</v>
-      </c>
-      <c r="B43" t="s">
-        <v>117</v>
-      </c>
-      <c r="C43" t="s">
-        <v>135</v>
-      </c>
-      <c r="D43" t="s">
-        <v>94</v>
-      </c>
-      <c r="E43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F43" t="s">
-        <v>130</v>
-      </c>
-      <c r="G43">
-        <v>2020</v>
-      </c>
-      <c r="H43" t="s">
-        <v>125</v>
-      </c>
-      <c r="I43" t="s">
-        <v>131</v>
-      </c>
-      <c r="J43" t="s">
-        <v>131</v>
-      </c>
-      <c r="K43" t="s">
-        <v>131</v>
-      </c>
-      <c r="L43">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44" t="s">
-        <v>117</v>
-      </c>
-      <c r="C44" t="s">
-        <v>135</v>
-      </c>
-      <c r="D44" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" t="s">
-        <v>130</v>
-      </c>
-      <c r="G44">
-        <v>2030</v>
-      </c>
-      <c r="H44" t="s">
-        <v>125</v>
-      </c>
-      <c r="I44" t="s">
-        <v>131</v>
-      </c>
-      <c r="J44" t="s">
-        <v>131</v>
-      </c>
-      <c r="K44" t="s">
-        <v>131</v>
-      </c>
-      <c r="L44">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>116</v>
-      </c>
-      <c r="B45" t="s">
-        <v>117</v>
-      </c>
-      <c r="C45" t="s">
-        <v>135</v>
-      </c>
-      <c r="D45" t="s">
-        <v>94</v>
-      </c>
-      <c r="E45" t="s">
-        <v>84</v>
-      </c>
-      <c r="F45" t="s">
-        <v>130</v>
-      </c>
-      <c r="G45">
-        <v>2040</v>
-      </c>
-      <c r="H45" t="s">
-        <v>125</v>
-      </c>
-      <c r="I45" t="s">
-        <v>131</v>
-      </c>
-      <c r="J45" t="s">
-        <v>131</v>
-      </c>
-      <c r="K45" t="s">
-        <v>131</v>
-      </c>
-      <c r="L45">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>116</v>
-      </c>
-      <c r="B46" t="s">
-        <v>117</v>
-      </c>
-      <c r="C46" t="s">
-        <v>135</v>
-      </c>
-      <c r="D46" t="s">
-        <v>94</v>
-      </c>
-      <c r="E46" t="s">
-        <v>84</v>
-      </c>
-      <c r="F46" t="s">
-        <v>130</v>
-      </c>
-      <c r="G46">
-        <v>2050</v>
-      </c>
-      <c r="H46" t="s">
-        <v>125</v>
-      </c>
-      <c r="I46" t="s">
-        <v>131</v>
-      </c>
-      <c r="J46" t="s">
-        <v>131</v>
-      </c>
-      <c r="K46" t="s">
-        <v>131</v>
-      </c>
-      <c r="L46">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>116</v>
-      </c>
-      <c r="B47" t="s">
-        <v>117</v>
-      </c>
-      <c r="C47" t="s">
-        <v>135</v>
-      </c>
-      <c r="D47" t="s">
-        <v>102</v>
-      </c>
-      <c r="E47" t="s">
-        <v>84</v>
-      </c>
-      <c r="F47" t="s">
-        <v>130</v>
-      </c>
-      <c r="G47">
-        <v>2018</v>
-      </c>
-      <c r="H47" t="s">
-        <v>125</v>
-      </c>
-      <c r="I47" t="s">
-        <v>131</v>
-      </c>
-      <c r="J47" t="s">
-        <v>131</v>
-      </c>
-      <c r="K47" t="s">
-        <v>131</v>
-      </c>
-      <c r="L47">
-        <v>0.95484143461821203</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>116</v>
-      </c>
-      <c r="B48" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" t="s">
-        <v>135</v>
-      </c>
-      <c r="D48" t="s">
-        <v>102</v>
-      </c>
-      <c r="E48" t="s">
-        <v>84</v>
-      </c>
-      <c r="F48" t="s">
-        <v>130</v>
-      </c>
-      <c r="G48">
-        <v>2020</v>
-      </c>
-      <c r="H48" t="s">
-        <v>125</v>
-      </c>
-      <c r="I48" t="s">
-        <v>131</v>
-      </c>
-      <c r="J48" t="s">
-        <v>131</v>
-      </c>
-      <c r="K48" t="s">
-        <v>131</v>
-      </c>
-      <c r="L48">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>116</v>
-      </c>
-      <c r="B49" t="s">
-        <v>117</v>
-      </c>
-      <c r="C49" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" t="s">
-        <v>102</v>
-      </c>
-      <c r="E49" t="s">
-        <v>84</v>
-      </c>
-      <c r="F49" t="s">
-        <v>130</v>
-      </c>
-      <c r="G49">
-        <v>2030</v>
-      </c>
-      <c r="H49" t="s">
-        <v>125</v>
-      </c>
-      <c r="I49" t="s">
-        <v>131</v>
-      </c>
-      <c r="J49" t="s">
-        <v>131</v>
-      </c>
-      <c r="K49" t="s">
-        <v>131</v>
-      </c>
-      <c r="L49">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>116</v>
-      </c>
-      <c r="B50" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" t="s">
-        <v>135</v>
-      </c>
-      <c r="D50" t="s">
-        <v>102</v>
-      </c>
-      <c r="E50" t="s">
-        <v>84</v>
-      </c>
-      <c r="F50" t="s">
-        <v>130</v>
-      </c>
-      <c r="G50">
-        <v>2040</v>
-      </c>
-      <c r="H50" t="s">
-        <v>125</v>
-      </c>
-      <c r="I50" t="s">
-        <v>131</v>
-      </c>
-      <c r="J50" t="s">
-        <v>131</v>
-      </c>
-      <c r="K50" t="s">
-        <v>131</v>
-      </c>
-      <c r="L50">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>116</v>
-      </c>
-      <c r="B51" t="s">
-        <v>117</v>
-      </c>
-      <c r="C51" t="s">
-        <v>135</v>
-      </c>
-      <c r="D51" t="s">
-        <v>102</v>
-      </c>
-      <c r="E51" t="s">
-        <v>84</v>
-      </c>
-      <c r="F51" t="s">
-        <v>130</v>
-      </c>
-      <c r="G51">
-        <v>2050</v>
-      </c>
-      <c r="H51" t="s">
-        <v>125</v>
-      </c>
-      <c r="I51" t="s">
-        <v>131</v>
-      </c>
-      <c r="J51" t="s">
-        <v>131</v>
-      </c>
-      <c r="K51" t="s">
-        <v>131</v>
-      </c>
-      <c r="L51">
-        <v>0.9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F0F7499-A5CE-4374-995E-DC72D788363A}">
   <dimension ref="A3:AD37"/>
   <sheetViews>
@@ -3898,12 +1890,74 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
+  <dimension ref="B2:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G3" s="11" t="str">
+        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH29" sqref="AH29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4459,7 +2513,7 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="M10" s="9"/>
       <c r="AL10" t="s">
@@ -4611,7 +2665,7 @@
         <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12">
         <v>2018</v>
@@ -4717,7 +2771,7 @@
         <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E13">
         <v>2018</v>
@@ -4823,7 +2877,7 @@
         <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14">
         <v>2018</v>
@@ -4923,7 +2977,7 @@
         <v>84</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E15">
         <v>2018</v>
@@ -5023,7 +3077,7 @@
         <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E16">
         <v>2018</v>
@@ -5123,7 +3177,7 @@
         <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -5223,7 +3277,7 @@
         <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -5329,7 +3383,7 @@
         <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -5435,7 +3489,7 @@
         <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -5541,7 +3595,7 @@
         <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -5644,10 +3698,10 @@
     </row>
     <row r="22" spans="3:39" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="D22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E22">
         <v>2018</v>
@@ -5734,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="AH22" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="AI22" t="str">
         <f>AL18</f>
@@ -5752,7 +3806,7 @@
         <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23">
         <v>2030</v>
@@ -5839,7 +3893,7 @@
         <v>0</v>
       </c>
       <c r="AH23" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="AI23" t="str">
         <f>AL21</f>
@@ -5856,7 +3910,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5919,7 +3973,7 @@
         <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>17</v>
@@ -5945,7 +3999,7 @@
         <v>2018</v>
       </c>
       <c r="J6" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K6" s="20">
         <v>4.5158565381788203E-2</v>
@@ -5994,7 +4048,7 @@
         <v>2020</v>
       </c>
       <c r="J8" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K8" s="20">
         <v>0.05</v>
@@ -6045,7 +4099,7 @@
         <v>2030</v>
       </c>
       <c r="J10" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K10" s="20">
         <v>0.1</v>
@@ -6095,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K12" s="21"/>
       <c r="L12" s="21">
@@ -6126,7 +4180,7 @@
         <v>2018</v>
       </c>
       <c r="J13" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K13">
         <v>0.15</v>
@@ -6180,7 +4234,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K15" s="21"/>
       <c r="L15" s="21">
@@ -6205,7 +4259,7 @@
         <v>2018</v>
       </c>
       <c r="J16" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -6248,7 +4302,7 @@
         <v>2020</v>
       </c>
       <c r="J18" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K18">
         <v>0.01</v>
@@ -6293,7 +4347,7 @@
         <v>2030</v>
       </c>
       <c r="J20" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K20">
         <v>0.5</v>
@@ -6344,7 +4398,7 @@
         <v>2040</v>
       </c>
       <c r="J22" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K22">
         <v>0.7</v>
@@ -6395,7 +4449,7 @@
         <v>2050</v>
       </c>
       <c r="J24" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K24">
         <v>0.9</v>
@@ -6456,7 +4510,7 @@
         <v>2018</v>
       </c>
       <c r="J27" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K27">
         <v>0.5</v>
@@ -6498,7 +4552,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="21" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K29" s="21"/>
       <c r="L29" s="21">
@@ -6523,7 +4577,7 @@
         <v>2018</v>
       </c>
       <c r="J30" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K30" s="20">
         <v>4.0877873467079801E-2</v>
@@ -6566,7 +4620,7 @@
         <v>2020</v>
       </c>
       <c r="J32" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K32" s="20">
         <v>5.1152531327863002E-2</v>
@@ -6605,7 +4659,7 @@
         <v>2030</v>
       </c>
       <c r="J34" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K34" s="20">
         <v>0.1</v>
@@ -6643,7 +4697,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K36" s="21"/>
       <c r="L36" s="21">
@@ -6657,7 +4711,7 @@
         <v>UC_T-OTH_CON00_Max_TRADSB</v>
       </c>
       <c r="D37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="G37" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,$P$10,$P$14)</f>
@@ -6667,7 +4721,7 @@
         <v>2018</v>
       </c>
       <c r="J37" s="22" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K37">
         <f>K38-1</f>
@@ -6709,7 +4763,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K39" s="21"/>
       <c r="L39" s="21">
@@ -6723,7 +4777,7 @@
         <v>UC_T-OTH_CON00_Min_TRAGSE</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="G40" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,$P$7,$P$11)</f>
@@ -6797,7 +4851,7 @@
         <v>UC_T-OTH_NEW_Min_TRANGB</v>
       </c>
       <c r="D43" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="G43" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,$P$9,$P$13)</f>
@@ -6807,7 +4861,7 @@
         <v>2018</v>
       </c>
       <c r="J43" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K43">
         <f>K44-1</f>
@@ -6839,7 +4893,7 @@
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="G45" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,$P$9,$P$13)</f>
@@ -6849,7 +4903,7 @@
         <v>2030</v>
       </c>
       <c r="J45" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K45">
         <f>K46-1</f>
@@ -6895,7 +4949,7 @@
         <v>0</v>
       </c>
       <c r="J47" s="21" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K47" s="21"/>
       <c r="L47" s="21">

</xml_diff>

<commit_message>
Re-introduce geothermal and add regionalisation where missing
- limit NCAP_BND for geothermal to 0 until costs are reviewed
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4A7955-DCC7-4BF4-86FD-C5F6FB3DA609}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB2A086-C04A-4EC0-8933-8F420D243C47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
-    <sheet name="HET" sheetId="19" r:id="rId2"/>
+    <sheet name="PWR" sheetId="19" r:id="rId2"/>
     <sheet name="TRA" sheetId="2" r:id="rId3"/>
     <sheet name="UCT_TRA" sheetId="18" r:id="rId4"/>
     <sheet name="UPD_biogas" sheetId="11" r:id="rId5"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="126">
   <si>
     <t>UC_N</t>
   </si>
@@ -491,6 +491,12 @@
   </si>
   <si>
     <t>HETD</t>
+  </si>
+  <si>
+    <t>PWR-GEO</t>
+  </si>
+  <si>
+    <t>NCAP_BND</t>
   </si>
 </sst>
 </file>
@@ -768,7 +774,7 @@
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000010C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000010C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1892,20 +1898,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
-  <dimension ref="B2:I4"/>
+  <dimension ref="B2:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
@@ -1933,7 +1942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>89</v>
       </c>
@@ -1945,6 +1954,77 @@
       </c>
       <c r="I4" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G8" s="11" t="str">
+        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9">
+        <v>2018</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1956,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:AI11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Feed HETD to AGR and COM in VT files
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F400A99-9206-474A-A576-75E197FC564F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAF0C4B-C151-4BC2-9421-1B4F7008833B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -389,9 +389,6 @@
     <t>~TFM_INS</t>
   </si>
   <si>
-    <t>FT-*HET</t>
-  </si>
-  <si>
     <t>HETD</t>
   </si>
   <si>
@@ -399,6 +396,9 @@
   </si>
   <si>
     <t>NCAP_BND</t>
+  </si>
+  <si>
+    <t>FT-RSDHET</t>
   </si>
 </sst>
 </file>
@@ -1798,12 +1798,13 @@
   <dimension ref="B2:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
@@ -1847,10 +1848,10 @@
         <v>88</v>
       </c>
       <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" t="s">
         <v>90</v>
-      </c>
-      <c r="I4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -1892,7 +1893,7 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9">
         <v>2018</v>
@@ -1904,12 +1905,12 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1921,7 +1922,7 @@
         <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Temporarily limit availability of forestry residues to 0
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAF0C4B-C151-4BC2-9421-1B4F7008833B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784374A4-F253-4288-B245-BE8ABC5505B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
-    <sheet name="PWR" sheetId="19" r:id="rId2"/>
-    <sheet name="UPD_biogas" sheetId="11" r:id="rId3"/>
-    <sheet name="UCT_biogas" sheetId="1" r:id="rId4"/>
+    <sheet name="AGR" sheetId="20" r:id="rId2"/>
+    <sheet name="PWR" sheetId="19" r:id="rId3"/>
+    <sheet name="UPD_biogas" sheetId="11" r:id="rId4"/>
+    <sheet name="UCT_biogas" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
   <si>
     <t>UC_N</t>
   </si>
@@ -399,6 +400,12 @@
   </si>
   <si>
     <t>FT-RSDHET</t>
+  </si>
+  <si>
+    <t>ACT_BND</t>
+  </si>
+  <si>
+    <t>ABIOFRSR*</t>
   </si>
 </sst>
 </file>
@@ -1794,11 +1801,96 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FEE988-9CBB-45F8-B07F-A9EAC00FE4CD}">
+  <dimension ref="B2:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G3" s="11" t="str">
+        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4">
+        <v>2018</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
   <dimension ref="B2:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,7 +2022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -2022,7 +2114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add an i/e rule to biomass potentials and disallow imports of WPE and WCH above 2018 levels
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784374A4-F253-4288-B245-BE8ABC5505B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5665764E-01BC-4437-BFCF-4DA736CE4BF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
-    <sheet name="AGR" sheetId="20" r:id="rId2"/>
+    <sheet name="IRE" sheetId="20" r:id="rId2"/>
     <sheet name="PWR" sheetId="19" r:id="rId3"/>
     <sheet name="UPD_biogas" sheetId="11" r:id="rId4"/>
     <sheet name="UCT_biogas" sheetId="1" r:id="rId5"/>
@@ -53,6 +53,29 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gary Goldstein</author>
+  </authors>
+  <commentList>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{9C56C09D-A62A-49BE-9ADB-AE1288CDCD1F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
@@ -98,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="99">
   <si>
     <t>UC_N</t>
   </si>
@@ -402,10 +425,19 @@
     <t>FT-RSDHET</t>
   </si>
   <si>
-    <t>ACT_BND</t>
-  </si>
-  <si>
-    <t>ABIOFRSR*</t>
+    <t>CAP_BND</t>
+  </si>
+  <si>
+    <t>IMPBIOWPE_S2</t>
+  </si>
+  <si>
+    <t>IMPBIOWPE_S3</t>
+  </si>
+  <si>
+    <t>IMPBIOWCH_S2</t>
+  </si>
+  <si>
+    <t>IMPBIOWCH_S3</t>
   </si>
 </sst>
 </file>
@@ -1801,21 +1833,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FEE988-9CBB-45F8-B07F-A9EAC00FE4CD}">
-  <dimension ref="B2:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A47D8E2-EF32-40FF-8372-26BFA87CC2D3}">
+  <dimension ref="B2:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
@@ -1828,60 +1866,166 @@
       <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="11" t="str">
+      <c r="F3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G3" s="11" t="str">
+      <c r="I3" s="11" t="str">
         <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>94</v>
       </c>
       <c r="E4">
         <v>2018</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>94</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>5</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>5</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6">
+        <v>2018</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="K7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8">
+        <v>2018</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10">
+        <v>2018</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1890,7 +2034,7 @@
   <dimension ref="B2:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:J10"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,7 +2171,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="B2" sqref="B2:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Apply some temp fixes and clean up the file
fixes:
- limit solar PV in SRV to 0.1 GW;
- move NCAP_START of most multi-fuel techs in RSD to 2200
- move NCAP_START of wave to 2200

clean-up:
 - remove 0 import bound on some bio, because bio is limited by a separate scenario
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5665764E-01BC-4437-BFCF-4DA736CE4BF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A8252D-01DF-459C-A6EA-F1432614E087}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
-    <sheet name="IRE" sheetId="20" r:id="rId2"/>
-    <sheet name="PWR" sheetId="19" r:id="rId3"/>
-    <sheet name="UPD_biogas" sheetId="11" r:id="rId4"/>
-    <sheet name="UCT_biogas" sheetId="1" r:id="rId5"/>
+    <sheet name="SRV" sheetId="21" r:id="rId2"/>
+    <sheet name="RSD" sheetId="22" r:id="rId3"/>
+    <sheet name="PWR" sheetId="19" r:id="rId4"/>
+    <sheet name="UPD_biogas" sheetId="11" r:id="rId5"/>
+    <sheet name="UCT_biogas" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -58,7 +59,7 @@
     <author>Gary Goldstein</author>
   </authors>
   <commentList>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{9C56C09D-A62A-49BE-9ADB-AE1288CDCD1F}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{0021F6E5-21A7-4C1D-B1BF-8245492E85D8}">
       <text>
         <r>
           <rPr>
@@ -76,6 +77,29 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gary Goldstein</author>
+  </authors>
+  <commentList>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{72AB0CFC-898D-4B3D-B9B0-FC3C4E8CA607}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
@@ -121,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
   <si>
     <t>UC_N</t>
   </si>
@@ -428,16 +452,22 @@
     <t>CAP_BND</t>
   </si>
   <si>
-    <t>IMPBIOWPE_S2</t>
-  </si>
-  <si>
-    <t>IMPBIOWPE_S3</t>
-  </si>
-  <si>
-    <t>IMPBIOWCH_S2</t>
-  </si>
-  <si>
-    <t>IMPBIOWCH_S3</t>
+    <t>* Unit</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>COMPVELC_01</t>
+  </si>
+  <si>
+    <t>R*SOL_HP*</t>
+  </si>
+  <si>
+    <t>R*_N2,R*_N3,-R*HP*,-R*HET*</t>
+  </si>
+  <si>
+    <t>P*WAV*</t>
   </si>
 </sst>
 </file>
@@ -555,7 +585,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -622,6 +652,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -630,7 +671,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -660,6 +701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1833,16 +1875,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A47D8E2-EF32-40FF-8372-26BFA87CC2D3}">
-  <dimension ref="B2:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A155980F-6689-4ADE-B1F2-DEFB665B2049}">
+  <dimension ref="B2:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
@@ -1888,139 +1930,63 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4">
-        <v>2018</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="B4" s="20" t="s">
         <v>95</v>
       </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
       <c r="D5" t="s">
         <v>94</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>2020</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <f>H5</f>
+        <v>0.1</v>
       </c>
       <c r="K5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
       <c r="D6" t="s">
         <v>94</v>
       </c>
       <c r="E6">
-        <v>2018</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <f>H6</f>
+        <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="K7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8">
-        <v>2018</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-      <c r="I9">
-        <v>5</v>
-      </c>
-      <c r="K9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10">
-        <v>2018</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>5</v>
-      </c>
-      <c r="K11" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2030,11 +1996,102 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB162A2-2D25-4675-8312-87FE93E3B4EE}">
+  <dimension ref="B2:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="I3" s="11" t="str">
+        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4">
+        <v>2200</v>
+      </c>
+      <c r="I4">
+        <f>H4</f>
+        <v>2200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5">
+        <v>2200</v>
+      </c>
+      <c r="I5">
+        <f>H5</f>
+        <v>2200</v>
+      </c>
+      <c r="K5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
-  <dimension ref="B2:M10"/>
+  <dimension ref="B2:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,6 +2195,7 @@
         <v>0</v>
       </c>
       <c r="G9">
+        <f>F9</f>
         <v>0</v>
       </c>
       <c r="H9" t="s">
@@ -2155,10 +2213,26 @@
         <v>5</v>
       </c>
       <c r="G10">
+        <f>F10</f>
         <v>5</v>
       </c>
       <c r="H10" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11">
+        <v>2200</v>
+      </c>
+      <c r="G11">
+        <f>F11</f>
+        <v>2200</v>
+      </c>
+      <c r="I11" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2166,7 +2240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -2258,12 +2332,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove TOPINS for HETD (included directly in RSD)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A8252D-01DF-459C-A6EA-F1432614E087}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14ADDE3-EE2D-4ED1-8959-17E61522AD7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
   <si>
     <t>UC_N</t>
   </si>
@@ -431,22 +431,13 @@
     <t>~TFM_TOPINS</t>
   </si>
   <si>
-    <t>IN</t>
-  </si>
-  <si>
     <t>~TFM_INS</t>
   </si>
   <si>
-    <t>HETD</t>
-  </si>
-  <si>
     <t>PWR-GEO</t>
   </si>
   <si>
     <t>NCAP_BND</t>
-  </si>
-  <si>
-    <t>FT-RSDHET</t>
   </si>
   <si>
     <t>CAP_BND</t>
@@ -1889,7 +1880,7 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="9"/>
@@ -1931,7 +1922,7 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -1939,10 +1930,10 @@
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
@@ -1952,7 +1943,7 @@
         <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E5">
         <v>2020</v>
@@ -1965,7 +1956,7 @@
         <v>0.1</v>
       </c>
       <c r="K5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -1973,7 +1964,7 @@
         <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1986,7 +1977,7 @@
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1999,7 +1990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB162A2-2D25-4675-8312-87FE93E3B4EE}">
   <dimension ref="B2:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
@@ -2062,7 +2053,7 @@
         <v>2200</v>
       </c>
       <c r="K4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -2077,7 +2068,7 @@
         <v>2200</v>
       </c>
       <c r="K5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2088,10 +2079,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
-  <dimension ref="B2:M11"/>
+  <dimension ref="B2:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,106 +2124,92 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="11" t="str">
+      <c r="F7" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G8" s="11" t="str">
+      <c r="G7" s="11" t="str">
         <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J7" s="12" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8">
+        <v>2018</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f>F8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E9">
-        <v>2018</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G9">
         <f>F9</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>2200</v>
       </c>
       <c r="G10">
         <f>F10</f>
-        <v>5</v>
-      </c>
-      <c r="H10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11">
         <v>2200</v>
       </c>
-      <c r="G11">
-        <f>F11</f>
-        <v>2200</v>
-      </c>
-      <c r="I11" t="s">
-        <v>100</v>
+      <c r="I10" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include emissions from fossils in RSD
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14ADDE3-EE2D-4ED1-8959-17E61522AD7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290E222B-48E5-4A29-884B-2453F485C3FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -80,6 +80,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
+    <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
     <comment ref="I2" authorId="0" shapeId="0" xr:uid="{72AB0CFC-898D-4B3D-B9B0-FC3C4E8CA607}">
@@ -92,6 +93,20 @@
             <family val="2"/>
           </rPr>
           <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="1" shapeId="0" xr:uid="{6084453E-3A70-4BA0-9471-3F6909BFC378}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insert Table</t>
         </r>
       </text>
     </comment>
@@ -145,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="112">
   <si>
     <t>UC_N</t>
   </si>
@@ -460,12 +475,54 @@
   <si>
     <t>P*WAV*</t>
   </si>
+  <si>
+    <t>RSDCOA</t>
+  </si>
+  <si>
+    <t>RSDPEA</t>
+  </si>
+  <si>
+    <t>kt/PJ</t>
+  </si>
+  <si>
+    <t>RSDCO2</t>
+  </si>
+  <si>
+    <t>RSDCH4</t>
+  </si>
+  <si>
+    <t>RSDSO2N</t>
+  </si>
+  <si>
+    <t>RSDPM10</t>
+  </si>
+  <si>
+    <t>RSDPM25</t>
+  </si>
+  <si>
+    <t>RSDLPG</t>
+  </si>
+  <si>
+    <t>RSDKER</t>
+  </si>
+  <si>
+    <t>RSDGAS</t>
+  </si>
+  <si>
+    <t>Other_indexes</t>
+  </si>
+  <si>
+    <t>*Unit</t>
+  </si>
+  <si>
+    <t>FLO_EMIS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,8 +582,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -573,6 +656,12 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -662,7 +751,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -693,6 +782,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1988,10 +2084,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB162A2-2D25-4675-8312-87FE93E3B4EE}">
-  <dimension ref="B2:K5"/>
+  <dimension ref="B2:AK33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,7 +2095,7 @@
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
@@ -2007,7 +2103,7 @@
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
@@ -2041,7 +2137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>79</v>
       </c>
@@ -2056,7 +2152,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>79</v>
       </c>
@@ -2069,6 +2165,667 @@
       </c>
       <c r="K5" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
+      <c r="AH9" s="22"/>
+      <c r="AI9" s="22"/>
+      <c r="AJ9" s="22"/>
+      <c r="AK9" s="22"/>
+    </row>
+    <row r="10" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G10" s="11" t="str">
+        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11">
+        <v>97.115822433347077</v>
+      </c>
+      <c r="G11" s="22">
+        <f>F11</f>
+        <v>97.115822433347077</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" s="22" t="str">
+        <f t="shared" ref="J11:J16" si="0">H11</f>
+        <v>RSDCOA</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="F12">
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="G12" s="22">
+        <f t="shared" ref="G12:G33" si="1">F12</f>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>RSDCOA</v>
+      </c>
+      <c r="K12" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13">
+        <v>1.4999999999999998E-3</v>
+      </c>
+      <c r="G13" s="22">
+        <f t="shared" si="1"/>
+        <v>1.4999999999999998E-3</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>RSDCOA</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14">
+        <v>0.31384830276066084</v>
+      </c>
+      <c r="G14" s="22">
+        <f t="shared" si="1"/>
+        <v>0.31384830276066084</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>RSDCOA</v>
+      </c>
+      <c r="K14" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="D15" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15">
+        <v>0.30918718935332451</v>
+      </c>
+      <c r="G15" s="22">
+        <f t="shared" si="1"/>
+        <v>0.30918718935332451</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15" t="s">
+        <v>105</v>
+      </c>
+      <c r="J15" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>RSDCOA</v>
+      </c>
+      <c r="K15" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="D16" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16">
+        <v>104</v>
+      </c>
+      <c r="G16" s="22">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J16" s="22" t="str">
+        <f t="shared" ref="J16:J33" si="2">H16</f>
+        <v>RSDPEA</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D17" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17">
+        <v>0.3</v>
+      </c>
+      <c r="G17" s="22">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDPEA</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18">
+        <v>1.4E-3</v>
+      </c>
+      <c r="G18" s="22">
+        <f t="shared" si="1"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDPEA</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D19" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19">
+        <v>63.7</v>
+      </c>
+      <c r="G19" s="22">
+        <f t="shared" si="1"/>
+        <v>63.7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19" t="s">
+        <v>101</v>
+      </c>
+      <c r="J19" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDLPG</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D20" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G20" s="22">
+        <f t="shared" si="1"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I20" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDLPG</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D21" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21">
+        <v>1E-4</v>
+      </c>
+      <c r="G21" s="22">
+        <f t="shared" si="1"/>
+        <v>1E-4</v>
+      </c>
+      <c r="H21" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDLPG</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D22" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22">
+        <v>3.609253890302349E-3</v>
+      </c>
+      <c r="G22" s="22">
+        <f t="shared" si="1"/>
+        <v>3.609253890302349E-3</v>
+      </c>
+      <c r="H22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDLPG</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23">
+        <v>3.609253890302349E-3</v>
+      </c>
+      <c r="G23" s="22">
+        <f t="shared" si="1"/>
+        <v>3.609253890302349E-3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" t="s">
+        <v>105</v>
+      </c>
+      <c r="J23" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDLPG</v>
+      </c>
+      <c r="K23" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="G24" s="22">
+        <f t="shared" si="1"/>
+        <v>71.400000000000006</v>
+      </c>
+      <c r="H24" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" t="s">
+        <v>101</v>
+      </c>
+      <c r="J24" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDKER</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D25" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25">
+        <v>0.01</v>
+      </c>
+      <c r="G25" s="22">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="H25" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDKER</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G26" s="22">
+        <f t="shared" si="1"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" t="s">
+        <v>103</v>
+      </c>
+      <c r="J26" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDKER</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27">
+        <v>3.1602980079786249E-3</v>
+      </c>
+      <c r="G27" s="22">
+        <f t="shared" si="1"/>
+        <v>3.1602980079786249E-3</v>
+      </c>
+      <c r="H27" t="s">
+        <v>107</v>
+      </c>
+      <c r="I27" t="s">
+        <v>104</v>
+      </c>
+      <c r="J27" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDKER</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D28" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F28">
+        <v>3.1602980079786249E-3</v>
+      </c>
+      <c r="G28" s="22">
+        <f t="shared" si="1"/>
+        <v>3.1602980079786249E-3</v>
+      </c>
+      <c r="H28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" t="s">
+        <v>105</v>
+      </c>
+      <c r="J28" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDKER</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="G29" s="22">
+        <f t="shared" si="1"/>
+        <v>71.400000000000006</v>
+      </c>
+      <c r="H29" t="s">
+        <v>108</v>
+      </c>
+      <c r="I29" t="s">
+        <v>101</v>
+      </c>
+      <c r="J29" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDGAS</v>
+      </c>
+      <c r="K29" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D30" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30">
+        <v>0.01</v>
+      </c>
+      <c r="G30" s="22">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="H30" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" t="s">
+        <v>102</v>
+      </c>
+      <c r="J30" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDGAS</v>
+      </c>
+      <c r="K30" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D31" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G31" s="22">
+        <f t="shared" si="1"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H31" t="s">
+        <v>108</v>
+      </c>
+      <c r="I31" t="s">
+        <v>103</v>
+      </c>
+      <c r="J31" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDGAS</v>
+      </c>
+      <c r="K31" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D32" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32">
+        <v>3.1602980079786249E-3</v>
+      </c>
+      <c r="G32" s="22">
+        <f t="shared" si="1"/>
+        <v>3.1602980079786249E-3</v>
+      </c>
+      <c r="H32" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" t="s">
+        <v>104</v>
+      </c>
+      <c r="J32" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDGAS</v>
+      </c>
+      <c r="K32" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D33" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33">
+        <v>3.1602980079786249E-3</v>
+      </c>
+      <c r="G33" s="22">
+        <f t="shared" si="1"/>
+        <v>3.1602980079786249E-3</v>
+      </c>
+      <c r="H33" t="s">
+        <v>108</v>
+      </c>
+      <c r="I33" t="s">
+        <v>105</v>
+      </c>
+      <c r="J33" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>RSDGAS</v>
+      </c>
+      <c r="K33" s="25" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2081,7 +2838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
   <dimension ref="B2:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Move NCAP_START for CCS in PWR to 2030 and specify NCAP_ILED of 5 years
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290E222B-48E5-4A29-884B-2453F485C3FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6857AB9-A8FC-4F63-90FF-4E3C19BBE5EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="114">
   <si>
     <t>UC_N</t>
   </si>
@@ -516,6 +516,12 @@
   </si>
   <si>
     <t>FLO_EMIS</t>
+  </si>
+  <si>
+    <t>P*CCS*</t>
+  </si>
+  <si>
+    <t>NCAP_ILED</t>
   </si>
 </sst>
 </file>
@@ -2086,7 +2092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB162A2-2D25-4675-8312-87FE93E3B4EE}">
   <dimension ref="B2:AK33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
@@ -2262,7 +2268,7 @@
         <v>101</v>
       </c>
       <c r="J11" s="22" t="str">
-        <f t="shared" ref="J11:J16" si="0">H11</f>
+        <f t="shared" ref="J11:J15" si="0">H11</f>
         <v>RSDCOA</v>
       </c>
       <c r="K11" s="25" t="s">
@@ -2836,10 +2842,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
-  <dimension ref="B2:M10"/>
+  <dimension ref="B2:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2967,6 +2973,36 @@
       </c>
       <c r="I10" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11">
+        <v>2030</v>
+      </c>
+      <c r="G11">
+        <f>F11</f>
+        <v>2030</v>
+      </c>
+      <c r="I11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <f>F12</f>
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove temp fixes for RSD and update case definitions to include recent changes
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6857AB9-A8FC-4F63-90FF-4E3C19BBE5EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A1CEFE-43C7-415E-B2C7-9C404B84F0AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
     <sheet name="SRV" sheetId="21" r:id="rId2"/>
-    <sheet name="RSD" sheetId="22" r:id="rId3"/>
-    <sheet name="PWR" sheetId="19" r:id="rId4"/>
-    <sheet name="UPD_biogas" sheetId="11" r:id="rId5"/>
-    <sheet name="UCT_biogas" sheetId="1" r:id="rId6"/>
+    <sheet name="PWR" sheetId="19" r:id="rId3"/>
+    <sheet name="UPD_biogas" sheetId="11" r:id="rId4"/>
+    <sheet name="UCT_biogas" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -80,44 +79,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
-    <author>Maurizio Gargiulo</author>
-  </authors>
-  <commentList>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{72AB0CFC-898D-4B3D-B9B0-FC3C4E8CA607}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="1" shapeId="0" xr:uid="{6084453E-3A70-4BA0-9471-3F6909BFC378}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Insert Table</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Gary Goldstein</author>
   </authors>
   <commentList>
     <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
@@ -160,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
   <si>
     <t>UC_N</t>
   </si>
@@ -467,55 +428,7 @@
     <t>COMPVELC_01</t>
   </si>
   <si>
-    <t>R*SOL_HP*</t>
-  </si>
-  <si>
-    <t>R*_N2,R*_N3,-R*HP*,-R*HET*</t>
-  </si>
-  <si>
     <t>P*WAV*</t>
-  </si>
-  <si>
-    <t>RSDCOA</t>
-  </si>
-  <si>
-    <t>RSDPEA</t>
-  </si>
-  <si>
-    <t>kt/PJ</t>
-  </si>
-  <si>
-    <t>RSDCO2</t>
-  </si>
-  <si>
-    <t>RSDCH4</t>
-  </si>
-  <si>
-    <t>RSDSO2N</t>
-  </si>
-  <si>
-    <t>RSDPM10</t>
-  </si>
-  <si>
-    <t>RSDPM25</t>
-  </si>
-  <si>
-    <t>RSDLPG</t>
-  </si>
-  <si>
-    <t>RSDKER</t>
-  </si>
-  <si>
-    <t>RSDGAS</t>
-  </si>
-  <si>
-    <t>Other_indexes</t>
-  </si>
-  <si>
-    <t>*Unit</t>
-  </si>
-  <si>
-    <t>FLO_EMIS</t>
   </si>
   <si>
     <t>P*CCS*</t>
@@ -528,7 +441,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,34 +501,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -662,12 +549,6 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -757,7 +638,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -788,13 +669,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2089,763 +1963,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB162A2-2D25-4675-8312-87FE93E3B4EE}">
-  <dimension ref="B2:AK33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="11" t="str">
-        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
-        <v>IE</v>
-      </c>
-      <c r="I3" s="11" t="str">
-        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
-        <v>National</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4">
-        <v>2200</v>
-      </c>
-      <c r="I4">
-        <f>H4</f>
-        <v>2200</v>
-      </c>
-      <c r="K4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5">
-        <v>2200</v>
-      </c>
-      <c r="I5">
-        <f>H5</f>
-        <v>2200</v>
-      </c>
-      <c r="K5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="22"/>
-      <c r="X9" s="22"/>
-      <c r="Y9" s="22"/>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="22"/>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="22"/>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="22"/>
-      <c r="AG9" s="22"/>
-      <c r="AH9" s="22"/>
-      <c r="AI9" s="22"/>
-      <c r="AJ9" s="22"/>
-      <c r="AK9" s="22"/>
-    </row>
-    <row r="10" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="11" t="str">
-        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
-        <v>IE</v>
-      </c>
-      <c r="G10" s="11" t="str">
-        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
-        <v>National</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="K10" s="24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11">
-        <v>97.115822433347077</v>
-      </c>
-      <c r="G11" s="22">
-        <f>F11</f>
-        <v>97.115822433347077</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" t="s">
-        <v>101</v>
-      </c>
-      <c r="J11" s="22" t="str">
-        <f t="shared" ref="J11:J15" si="0">H11</f>
-        <v>RSDCOA</v>
-      </c>
-      <c r="K11" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="22"/>
-      <c r="F12">
-        <v>0.29999999999999993</v>
-      </c>
-      <c r="G12" s="22">
-        <f t="shared" ref="G12:G33" si="1">F12</f>
-        <v>0.29999999999999993</v>
-      </c>
-      <c r="H12" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="I12" t="s">
-        <v>102</v>
-      </c>
-      <c r="J12" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>RSDCOA</v>
-      </c>
-      <c r="K12" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="22"/>
-      <c r="F13">
-        <v>1.4999999999999998E-3</v>
-      </c>
-      <c r="G13" s="22">
-        <f t="shared" si="1"/>
-        <v>1.4999999999999998E-3</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="I13" t="s">
-        <v>103</v>
-      </c>
-      <c r="J13" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>RSDCOA</v>
-      </c>
-      <c r="K13" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14">
-        <v>0.31384830276066084</v>
-      </c>
-      <c r="G14" s="22">
-        <f t="shared" si="1"/>
-        <v>0.31384830276066084</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" t="s">
-        <v>104</v>
-      </c>
-      <c r="J14" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>RSDCOA</v>
-      </c>
-      <c r="K14" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D15" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15">
-        <v>0.30918718935332451</v>
-      </c>
-      <c r="G15" s="22">
-        <f t="shared" si="1"/>
-        <v>0.30918718935332451</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" t="s">
-        <v>105</v>
-      </c>
-      <c r="J15" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>RSDCOA</v>
-      </c>
-      <c r="K15" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D16" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F16">
-        <v>104</v>
-      </c>
-      <c r="G16" s="22">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="I16" t="s">
-        <v>101</v>
-      </c>
-      <c r="J16" s="22" t="str">
-        <f t="shared" ref="J16:J33" si="2">H16</f>
-        <v>RSDPEA</v>
-      </c>
-      <c r="K16" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D17" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17">
-        <v>0.3</v>
-      </c>
-      <c r="G17" s="22">
-        <f t="shared" si="1"/>
-        <v>0.3</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="I17" t="s">
-        <v>102</v>
-      </c>
-      <c r="J17" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDPEA</v>
-      </c>
-      <c r="K17" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D18" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F18">
-        <v>1.4E-3</v>
-      </c>
-      <c r="G18" s="22">
-        <f t="shared" si="1"/>
-        <v>1.4E-3</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="I18" t="s">
-        <v>103</v>
-      </c>
-      <c r="J18" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDPEA</v>
-      </c>
-      <c r="K18" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D19" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F19">
-        <v>63.7</v>
-      </c>
-      <c r="G19" s="22">
-        <f t="shared" si="1"/>
-        <v>63.7</v>
-      </c>
-      <c r="H19" t="s">
-        <v>106</v>
-      </c>
-      <c r="I19" t="s">
-        <v>101</v>
-      </c>
-      <c r="J19" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDLPG</v>
-      </c>
-      <c r="K19" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D20" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F20">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G20" s="22">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="H20" t="s">
-        <v>106</v>
-      </c>
-      <c r="I20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J20" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDLPG</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D21" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F21">
-        <v>1E-4</v>
-      </c>
-      <c r="G21" s="22">
-        <f t="shared" si="1"/>
-        <v>1E-4</v>
-      </c>
-      <c r="H21" t="s">
-        <v>106</v>
-      </c>
-      <c r="I21" t="s">
-        <v>103</v>
-      </c>
-      <c r="J21" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDLPG</v>
-      </c>
-      <c r="K21" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D22" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F22">
-        <v>3.609253890302349E-3</v>
-      </c>
-      <c r="G22" s="22">
-        <f t="shared" si="1"/>
-        <v>3.609253890302349E-3</v>
-      </c>
-      <c r="H22" t="s">
-        <v>106</v>
-      </c>
-      <c r="I22" t="s">
-        <v>104</v>
-      </c>
-      <c r="J22" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDLPG</v>
-      </c>
-      <c r="K22" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D23" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23">
-        <v>3.609253890302349E-3</v>
-      </c>
-      <c r="G23" s="22">
-        <f t="shared" si="1"/>
-        <v>3.609253890302349E-3</v>
-      </c>
-      <c r="H23" t="s">
-        <v>106</v>
-      </c>
-      <c r="I23" t="s">
-        <v>105</v>
-      </c>
-      <c r="J23" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDLPG</v>
-      </c>
-      <c r="K23" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D24" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="G24" s="22">
-        <f t="shared" si="1"/>
-        <v>71.400000000000006</v>
-      </c>
-      <c r="H24" t="s">
-        <v>107</v>
-      </c>
-      <c r="I24" t="s">
-        <v>101</v>
-      </c>
-      <c r="J24" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDKER</v>
-      </c>
-      <c r="K24" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D25" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F25">
-        <v>0.01</v>
-      </c>
-      <c r="G25" s="22">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="H25" t="s">
-        <v>107</v>
-      </c>
-      <c r="I25" t="s">
-        <v>102</v>
-      </c>
-      <c r="J25" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDKER</v>
-      </c>
-      <c r="K25" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D26" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F26">
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="G26" s="22">
-        <f t="shared" si="1"/>
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="H26" t="s">
-        <v>107</v>
-      </c>
-      <c r="I26" t="s">
-        <v>103</v>
-      </c>
-      <c r="J26" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDKER</v>
-      </c>
-      <c r="K26" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F27">
-        <v>3.1602980079786249E-3</v>
-      </c>
-      <c r="G27" s="22">
-        <f t="shared" si="1"/>
-        <v>3.1602980079786249E-3</v>
-      </c>
-      <c r="H27" t="s">
-        <v>107</v>
-      </c>
-      <c r="I27" t="s">
-        <v>104</v>
-      </c>
-      <c r="J27" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDKER</v>
-      </c>
-      <c r="K27" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D28" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F28">
-        <v>3.1602980079786249E-3</v>
-      </c>
-      <c r="G28" s="22">
-        <f t="shared" si="1"/>
-        <v>3.1602980079786249E-3</v>
-      </c>
-      <c r="H28" t="s">
-        <v>107</v>
-      </c>
-      <c r="I28" t="s">
-        <v>105</v>
-      </c>
-      <c r="J28" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDKER</v>
-      </c>
-      <c r="K28" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D29" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F29">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="G29" s="22">
-        <f t="shared" si="1"/>
-        <v>71.400000000000006</v>
-      </c>
-      <c r="H29" t="s">
-        <v>108</v>
-      </c>
-      <c r="I29" t="s">
-        <v>101</v>
-      </c>
-      <c r="J29" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDGAS</v>
-      </c>
-      <c r="K29" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D30" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F30">
-        <v>0.01</v>
-      </c>
-      <c r="G30" s="22">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="H30" t="s">
-        <v>108</v>
-      </c>
-      <c r="I30" t="s">
-        <v>102</v>
-      </c>
-      <c r="J30" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDGAS</v>
-      </c>
-      <c r="K30" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D31" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F31">
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="G31" s="22">
-        <f t="shared" si="1"/>
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="H31" t="s">
-        <v>108</v>
-      </c>
-      <c r="I31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J31" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDGAS</v>
-      </c>
-      <c r="K31" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D32" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F32">
-        <v>3.1602980079786249E-3</v>
-      </c>
-      <c r="G32" s="22">
-        <f t="shared" si="1"/>
-        <v>3.1602980079786249E-3</v>
-      </c>
-      <c r="H32" t="s">
-        <v>108</v>
-      </c>
-      <c r="I32" t="s">
-        <v>104</v>
-      </c>
-      <c r="J32" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDGAS</v>
-      </c>
-      <c r="K32" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D33" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F33">
-        <v>3.1602980079786249E-3</v>
-      </c>
-      <c r="G33" s="22">
-        <f t="shared" si="1"/>
-        <v>3.1602980079786249E-3</v>
-      </c>
-      <c r="H33" t="s">
-        <v>108</v>
-      </c>
-      <c r="I33" t="s">
-        <v>105</v>
-      </c>
-      <c r="J33" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>RSDGAS</v>
-      </c>
-      <c r="K33" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
   <dimension ref="B2:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,7 +2094,7 @@
         <v>2200</v>
       </c>
       <c r="I10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -2987,12 +2109,12 @@
         <v>2030</v>
       </c>
       <c r="I11" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -3002,7 +2124,7 @@
         <v>5</v>
       </c>
       <c r="I12" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3010,11 +2132,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:K4"/>
     </sheetView>
   </sheetViews>
@@ -3102,7 +2224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Limit capacity of HPs by the number of new and retrofitted buildings
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A1CEFE-43C7-415E-B2C7-9C404B84F0AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605D7264-5DD7-406C-AC0B-49C1DF37BEEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
     <sheet name="SRV" sheetId="21" r:id="rId2"/>
     <sheet name="PWR" sheetId="19" r:id="rId3"/>
     <sheet name="UPD_biogas" sheetId="11" r:id="rId4"/>
-    <sheet name="UCT_biogas" sheetId="1" r:id="rId5"/>
+    <sheet name="RSD" sheetId="22" r:id="rId5"/>
+    <sheet name="UCT_biogas" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -121,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="112">
   <si>
     <t>UC_N</t>
   </si>
@@ -435,6 +436,48 @@
   </si>
   <si>
     <t>NCAP_ILED</t>
+  </si>
+  <si>
+    <t>R-BLD_AptN1,R-RTFT-Apt*</t>
+  </si>
+  <si>
+    <t>UC_CAP</t>
+  </si>
+  <si>
+    <t>RSDSH_Apt</t>
+  </si>
+  <si>
+    <t>R*HPN*,-R*GAS*</t>
+  </si>
+  <si>
+    <t>temp_UC_HP-CAP_RSD-DET</t>
+  </si>
+  <si>
+    <t>temp_UC_HP-CAP_RSD-ATT</t>
+  </si>
+  <si>
+    <t>temp_UC_HP-CAP_RSD-APT</t>
+  </si>
+  <si>
+    <t>R-BLD_DetN1,R-RTFT-Det*</t>
+  </si>
+  <si>
+    <t>R-BLD_AttN1,R-RTFT-Att*</t>
+  </si>
+  <si>
+    <t>RSDSH_Att</t>
+  </si>
+  <si>
+    <t>RSDSH_Det</t>
+  </si>
+  <si>
+    <t>Capacity of HPs is constrained by new and retrofitted apartments</t>
+  </si>
+  <si>
+    <t>Capacity of HPs is constrained by new and retrofitted attached buildings</t>
+  </si>
+  <si>
+    <t>Capacity of HPs is constrained by new and retrofitted detached buildings</t>
   </si>
 </sst>
 </file>
@@ -2136,7 +2179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:K4"/>
     </sheetView>
   </sheetViews>
@@ -2225,11 +2268,232 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6">
+        <v>2020</v>
+      </c>
+      <c r="I6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>2020</v>
+      </c>
+      <c r="J7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9">
+        <v>2020</v>
+      </c>
+      <c r="I9" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10">
+        <v>2020</v>
+      </c>
+      <c r="J10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12">
+        <v>2020</v>
+      </c>
+      <c r="I12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" t="s">
+        <v>108</v>
+      </c>
+      <c r="H13">
+        <v>2020</v>
+      </c>
+      <c r="J13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection sqref="A1:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Swap coefficients for buildings/retrofits and HPs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605D7264-5DD7-406C-AC0B-49C1DF37BEEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E8525F-5AC9-47FA-A964-2D9986DF5510}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -2272,7 +2272,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2350,13 +2350,13 @@
         <v>98</v>
       </c>
       <c r="H6">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="I6" t="s">
         <v>83</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -2373,10 +2373,10 @@
         <v>100</v>
       </c>
       <c r="H7">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="J7">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2398,13 +2398,13 @@
         <v>106</v>
       </c>
       <c r="H9">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="I9" t="s">
         <v>83</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -2421,10 +2421,10 @@
         <v>107</v>
       </c>
       <c r="H10">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="J10">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2443,13 +2443,13 @@
         <v>105</v>
       </c>
       <c r="H12">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="I12" t="s">
         <v>83</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -2466,10 +2466,10 @@
         <v>108</v>
       </c>
       <c r="H13">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="J13">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add fixes to SRV - constraint oil to 3PJ - remove hydrogen HP and DH - constraint the growth rate of HPs to 10% per annum - constraint the growth rate of boilers consuming biomass to 10% per annum
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\main-40\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61199A89-F648-496C-85CA-F1179FD7BCD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3367D6-AE6D-4493-B2EA-4B711DD65E2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -63,6 +63,19 @@
   </authors>
   <commentList>
     <comment ref="I2" authorId="0" shapeId="0" xr:uid="{0021F6E5-21A7-4C1D-B1BF-8245492E85D8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{BD84AB6D-75EC-4779-B9B3-091258269305}">
       <text>
         <r>
           <rPr>
@@ -148,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="236">
   <si>
     <t>UC_N</t>
   </si>
@@ -820,15 +833,73 @@
   <si>
     <t>TFM_Fill-R: w=RSDAFC; Hcol=Region</t>
   </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>C*DH</t>
+  </si>
+  <si>
+    <t>C*H2*HP</t>
+  </si>
+  <si>
+    <t>COM_BNDPRD</t>
+  </si>
+  <si>
+    <t>COMOIL</t>
+  </si>
+  <si>
+    <t>UC_ATTR</t>
+  </si>
+  <si>
+    <t>UC_CAP~RHS</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS~2018</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS~0</t>
+  </si>
+  <si>
+    <t>CAP, GROWTH</t>
+  </si>
+  <si>
+    <t>Public sector - maximum growth rate of HPs</t>
+  </si>
+  <si>
+    <t>UC-SRV-PS_MaxGrowthHPs</t>
+  </si>
+  <si>
+    <t>C*PS*HP</t>
+  </si>
+  <si>
+    <t>Commercial sector - maximum growth rate of HPs</t>
+  </si>
+  <si>
+    <t>UC-SRV-CS_MaxGrowthHPs</t>
+  </si>
+  <si>
+    <t>C*CS*HP</t>
+  </si>
+  <si>
+    <t>Services - maximum growth rate of biomass</t>
+  </si>
+  <si>
+    <t>UC-SRV-MaxGrowthBio</t>
+  </si>
+  <si>
+    <t>C*SBIO*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -909,8 +980,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -963,6 +1047,24 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1065,7 +1167,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1112,7 +1214,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1165,7 +1276,7 @@
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000010C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000010C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2289,18 +2400,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A155980F-6689-4ADE-B1F2-DEFB665B2049}">
-  <dimension ref="B2:K6"/>
+  <dimension ref="B2:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>88</v>
       </c>
@@ -2308,7 +2422,7 @@
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
@@ -2341,8 +2455,11 @@
       <c r="K3" s="12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>92</v>
       </c>
@@ -2359,8 +2476,9 @@
       </c>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="20"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>83</v>
       </c>
@@ -2381,7 +2499,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>83</v>
       </c>
@@ -2400,6 +2518,328 @@
       </c>
       <c r="K6" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7">
+        <v>2020</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="L8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="I16" s="11" t="str">
+        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>217</v>
+      </c>
+      <c r="H18">
+        <v>2200</v>
+      </c>
+      <c r="I18">
+        <v>2200</v>
+      </c>
+      <c r="K18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>217</v>
+      </c>
+      <c r="H19">
+        <v>2200</v>
+      </c>
+      <c r="I19">
+        <v>2200</v>
+      </c>
+      <c r="K19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K28" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="L28" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="M28" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="N28" s="31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="H29" s="30">
+        <v>2018</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="J29" s="30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K29" s="30">
+        <v>1</v>
+      </c>
+      <c r="L29" s="34">
+        <v>-0.5</v>
+      </c>
+      <c r="M29" s="30">
+        <v>5</v>
+      </c>
+      <c r="N29" s="30" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="H30" s="30">
+        <v>2018</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="J30" s="30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K30" s="30">
+        <v>1</v>
+      </c>
+      <c r="L30" s="34">
+        <v>-0.5</v>
+      </c>
+      <c r="M30" s="30">
+        <v>5</v>
+      </c>
+      <c r="N30" s="30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="H31" s="30">
+        <v>2018</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="J31" s="30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K31" s="30">
+        <v>1</v>
+      </c>
+      <c r="L31" s="34">
+        <v>-0.5</v>
+      </c>
+      <c r="M31" s="30">
+        <v>5</v>
+      </c>
+      <c r="N31" s="30" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2675,7 +3115,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2785,7 +3225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Disable SRV constraints in Temporary_Fixes
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C8AFBF-7488-41A7-99A1-BDC46A63B7FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DE4387-62A7-433E-8F57-75FAB6DC07E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="253">
   <si>
     <t>UC_N</t>
   </si>
@@ -2619,8 +2619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A155980F-6689-4ADE-B1F2-DEFB665B2049}">
   <dimension ref="B2:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2634,9 +2634,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
-        <v>88</v>
-      </c>
+      <c r="B2" s="7"/>
       <c r="I2" s="8"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
@@ -2780,9 +2778,7 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B15" s="7"/>
       <c r="I15" s="8"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -2906,9 +2902,7 @@
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
       <c r="H27" s="30"/>
-      <c r="I27" s="30" t="s">
-        <v>7</v>
-      </c>
+      <c r="I27" s="30"/>
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
       <c r="L27" s="30"/>
@@ -3444,8 +3438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
   <dimension ref="A1:S173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K87" sqref="K87"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Set a limit on DH grid to the 2018 value
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C481D7D8-5F36-4B7E-844F-39AC99D51A2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E28C18-8C01-4DB7-992F-FC273DB20C62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="235">
   <si>
     <t>UC_N</t>
   </si>
@@ -842,6 +842,12 @@
   </si>
   <si>
     <t>TS_Filter</t>
+  </si>
+  <si>
+    <t>HETC</t>
+  </si>
+  <si>
+    <t>*GRID*</t>
   </si>
 </sst>
 </file>
@@ -2622,10 +2628,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:L6"/>
+  <dimension ref="B3:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,6 +2734,92 @@
       <c r="I6" t="str">
         <f>I5</f>
         <v>IMPBIO*1G*2,IMPBIO*1G*3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G12" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13">
+        <v>2018</v>
+      </c>
+      <c r="F13">
+        <v>0.35</v>
+      </c>
+      <c r="G13">
+        <f>F13</f>
+        <v>0.35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>233</v>
+      </c>
+      <c r="I13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C14" t="str">
+        <f>C13</f>
+        <v>UP</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" ref="D14" si="1">D13</f>
+        <v>ACT_BND</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <f>F14</f>
+        <v>5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>233</v>
+      </c>
+      <c r="I14" t="str">
+        <f>I13</f>
+        <v>*GRID*</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Disallow S4 of 1G biodiesel(ethanol) import
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E28C18-8C01-4DB7-992F-FC273DB20C62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A7053A-52BD-457A-B706-AB5E3D0DEC18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -832,9 +832,6 @@
     <t>R-SW_Det_HVO_N1</t>
   </si>
   <si>
-    <t>IMPBIO*1G*2,IMPBIO*1G*3</t>
-  </si>
-  <si>
     <t>ACT_BND</t>
   </si>
   <si>
@@ -848,6 +845,9 @@
   </si>
   <si>
     <t>*GRID*</t>
+  </si>
+  <si>
+    <t>IMPBIO*1G*2,IMPBIO*1G*3,IMPBIO*1G*4</t>
   </si>
 </sst>
 </file>
@@ -2631,7 +2631,7 @@
   <dimension ref="B3:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2642,7 +2642,7 @@
     <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="7.42578125" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2682,10 +2682,10 @@
         <v>3</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -2693,7 +2693,7 @@
         <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E5">
         <v>2018</v>
@@ -2706,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="I6" t="str">
         <f>I5</f>
-        <v>IMPBIO*1G*2,IMPBIO*1G*3</v>
+        <v>IMPBIO*1G*2,IMPBIO*1G*3,IMPBIO*1G*4</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -2776,7 +2776,7 @@
         <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E13">
         <v>2018</v>
@@ -2789,10 +2789,10 @@
         <v>0.35</v>
       </c>
       <c r="H13" t="s">
+        <v>232</v>
+      </c>
+      <c r="I13" t="s">
         <v>233</v>
-      </c>
-      <c r="I13" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
@@ -2815,7 +2815,7 @@
         <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I14" t="str">
         <f>I13</f>

</xml_diff>